<commit_message>
added get_mut_list and mut_cutoffs
</commit_message>
<xml_diff>
--- a/Files on Freqs/Book1.xlsx
+++ b/Files on Freqs/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adibnzv/Desktop/DESKTOP/SCHOOL/PhD/Year 1/Semester 2/Python for Biologists/Final Project/PythonCourse_Final_Project/Files on Freqs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A66F1999-2B2F-7A4E-8859-B33BE3082ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377321B1-0891-8C42-A1E7-3687B03AF2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{47E8FB99-E631-0847-90B9-6D14DF24A723}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{47E8FB99-E631-0847-90B9-6D14DF24A723}"/>
   </bookViews>
   <sheets>
     <sheet name="Carmel" sheetId="1" r:id="rId1"/>
@@ -297,12 +297,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -317,9 +323,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +644,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F89D19-4D5E-6E43-95FD-8FFCC2EB4793}">
   <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A27" sqref="A19:A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,47 +841,47 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -939,17 +946,17 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1017,13 +1024,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2CFBA3-AD69-1C4F-804E-1386952F337B}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>